<commit_message>
Até a página 225
</commit_message>
<xml_diff>
--- a/Cap_04/ROC.xlsx
+++ b/Cap_04/ROC.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e8221224b16f74c/Área de Trabalho/Portifólio/Projetos-Packt/Cap_04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2C04E51-CF1F-4866-8310-DAD8E6470CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{B2C04E51-CF1F-4866-8310-DAD8E6470CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10909F05-9F7F-4CB2-9BFE-44B798EF9113}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6933056A-CA6E-4195-994F-1BB8EE37B145}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6933056A-CA6E-4195-994F-1BB8EE37B145}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>target</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>DELTA</t>
-  </si>
-  <si>
-    <t>SE(E(SE($D4&gt;=J$3;1;0)=1;$C4=1);"TP";SE(E(SE($D4&gt;=J$3;1;0)=1;$C4=0);"FP";SE(E(SE($D4&gt;=J$3;1;0)=0;$C4=0);"TN";"FN")))</t>
   </si>
   <si>
     <t>ONE</t>
@@ -155,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -170,10 +167,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -972,6 +966,11 @@
               <c:symbol val="none"/>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-ED08-47C0-9660-E4ECFAD3941E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="56"/>
@@ -979,6 +978,11 @@
               <c:symbol val="none"/>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-ED08-47C0-9660-E4ECFAD3941E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
@@ -3614,6 +3618,717 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>OPTIMAL THRESHOLD PROBA</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>predicted</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Planilha1!$D$4:$D$103</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.87917460461220731</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87694016290479582</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86797011787238543</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86595524226076415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85986664458974493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8463237017498767</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84593097515090998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84571889733537742</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84461273796741554</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84368409148019563</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83796019061669591</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.82943638742077919</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82889733184058156</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8002356640189463</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.77595082469774057</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7725483443109159</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.76642992686754197</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.76052178325780018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.74877325916405391</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74525343274217692</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.73509792530784568</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.71643845313201526</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.71410578795144652</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.71159287723557718</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.70771957404173891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.6919612142383158</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.69060209827893837</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.68773417672360138</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.68737038984428245</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.68626026907854087</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.67912901009569127</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.67037033618642783</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.66744081421714863</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.66093142003481353</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.65685293981652582</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.62695388114647077</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.62536704495092976</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.62209179193246711</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.61897775862776039</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.61844515358065077</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.61377188699284413</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.60159825535304856</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.60017987205705625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.5982672061223917</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.59281470805812109</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.58930559738785149</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.57638935237044342</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.56044683284418761</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.55463173514181308</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.54521688469739527</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5405115767618951</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.53108023350806055</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52695518551708276</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.51725879311664247</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.51520619327012718</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.50437853489565687</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.49799708219860989</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.49513040090680471</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.46923223310984041</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.46220733159359811</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.4582169282925691</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.45057653670187497</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.45036736485022272</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.44899274693212882</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.43631261987652131</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.43493074414547273</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.43240293537987229</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.42026274633744681</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.39409410005411988</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.39314176883318741</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.3925361340617225</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.38918683376256152</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.38675034267852498</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.37497064556824339</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.36749132332899198</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.36726631544187133</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.36709953716087401</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.35509619180686008</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.35454975518963822</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.35094332248268362</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.34173175023008862</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.34078333587274712</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.33996160754444349</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.32883573559615181</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.31544283214283553</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.29067688099197719</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.28242949295540581</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.274402700216416</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.25441446421327812</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.23522304847260189</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.23505383886836231</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.2159355695236084</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.209187610604435</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.2016386088891195</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.1731316695405202</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.1685558448107094</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.1600015944869726</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.15031009908856041</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.1165863831049371</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.1154746898385941</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5722-439C-AC54-98174AFA65A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1698543759"/>
+        <c:axId val="1698566799"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>THRS</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="diamond"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dPt>
+                  <c:idx val="0"/>
+                  <c:marker>
+                    <c:symbol val="triangle"/>
+                    <c:size val="6"/>
+                    <c:spPr>
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:ln w="9525">
+                        <a:solidFill>
+                          <a:schemeClr val="accent2"/>
+                        </a:solidFill>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                  </c:marker>
+                  <c:bubble3D val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000067-5722-439C-AC54-98174AFA65A1}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$A$78</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>74</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$D$78</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0000</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0.36749132332899198</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000064-5722-439C-AC54-98174AFA65A1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1698543759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1698566799"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:minorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1698566799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.9"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1698543759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3655,6 +4370,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4726,20 +5481,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>605790</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4768,16 +6039,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>456480</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>275505</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>111810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4802,6 +6073,154 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>273600</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>112762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75C44811-3268-F787-4986-E8BBE91844CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>532899</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>532899</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>10026</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector reto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A308E4A-D58F-571F-2127-3E417E630828}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16605083" y="10763250"/>
+          <a:ext cx="0" cy="3915276"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>391026</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>180473</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>50132</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>180473</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector reto 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CCCAD2A-C893-C7AA-09C0-B8C9071BE0E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12793579" y="13324973"/>
+          <a:ext cx="5163553" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5126,23 +6545,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646A7AD2-905A-4927-825C-6D7158EA0606}">
   <dimension ref="A3:AA220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L110" sqref="L110"/>
+    <sheetView tabSelected="1" topLeftCell="D55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M112" sqref="M112:M114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1"/>
+    <col min="20" max="22" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -5151,11 +6572,11 @@
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="2">
         <v>0.375</v>
@@ -5197,14 +6618,11 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="W3" s="2"/>
-      <c r="X3" t="s">
-        <v>12</v>
-      </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -5286,7 +6704,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5320,7 +6738,7 @@
         <v>TP</v>
       </c>
       <c r="K5" s="2" t="str">
-        <f t="shared" ref="J5:V68" si="6">IF(AND(IF($D5&gt;=K$3,1,0)=1,$C5=1),"TP",IF(AND(IF($D5&gt;=K$3,1,0)=1,$C5=0),"FP",IF(AND(IF($D5&gt;=K$3,1,0)=0,$C5=0),"TN","FN")))</f>
+        <f t="shared" ref="K5:V20" si="6">IF(AND(IF($D5&gt;=K$3,1,0)=1,$C5=1),"TP",IF(AND(IF($D5&gt;=K$3,1,0)=1,$C5=0),"FP",IF(AND(IF($D5&gt;=K$3,1,0)=0,$C5=0),"TN","FN")))</f>
         <v>TP</v>
       </c>
       <c r="L5" s="2" t="str">
@@ -5368,7 +6786,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5450,7 +6868,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5532,7 +6950,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -5614,7 +7032,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5696,7 +7114,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5778,7 +7196,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -5860,7 +7278,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -5942,7 +7360,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -6024,7 +7442,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -6106,7 +7524,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -6188,7 +7606,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -6270,7 +7688,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -6352,7 +7770,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -6434,7 +7852,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -6516,7 +7934,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -6598,7 +8016,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -6680,7 +8098,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -6762,7 +8180,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -6844,7 +8262,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -6926,7 +8344,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -7008,7 +8426,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -7090,7 +8508,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -7172,7 +8590,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -7254,7 +8672,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -7336,7 +8754,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -7418,7 +8836,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -7500,7 +8918,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
@@ -7582,7 +9000,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -7664,7 +9082,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
@@ -7746,7 +9164,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
@@ -7828,7 +9246,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
@@ -7910,7 +9328,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
@@ -7992,7 +9410,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
@@ -8074,7 +9492,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
@@ -8156,7 +9574,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
@@ -8238,7 +9656,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
@@ -8320,7 +9738,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
@@ -8402,7 +9820,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
@@ -8484,7 +9902,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40</v>
       </c>
@@ -8566,7 +9984,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>41</v>
       </c>
@@ -8648,7 +10066,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>42</v>
       </c>
@@ -8730,7 +10148,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>43</v>
       </c>
@@ -8812,7 +10230,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>44</v>
       </c>
@@ -8894,7 +10312,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>45</v>
       </c>
@@ -8976,7 +10394,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>46</v>
       </c>
@@ -9058,7 +10476,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>47</v>
       </c>
@@ -9140,7 +10558,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>48</v>
       </c>
@@ -9222,7 +10640,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>49</v>
       </c>
@@ -9304,7 +10722,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>50</v>
       </c>
@@ -9386,7 +10804,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>51</v>
       </c>
@@ -9468,7 +10886,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>52</v>
       </c>
@@ -9550,7 +10968,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>53</v>
       </c>
@@ -9632,7 +11050,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>54</v>
       </c>
@@ -9714,7 +11132,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>55</v>
       </c>
@@ -9796,7 +11214,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>56</v>
       </c>
@@ -9878,7 +11296,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>57</v>
       </c>
@@ -9960,7 +11378,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>58</v>
       </c>
@@ -10042,7 +11460,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>59</v>
       </c>
@@ -10124,7 +11542,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>60</v>
       </c>
@@ -10206,7 +11624,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>61</v>
       </c>
@@ -10288,7 +11706,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>62</v>
       </c>
@@ -10370,7 +11788,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>63</v>
       </c>
@@ -10452,7 +11870,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>64</v>
       </c>
@@ -10534,7 +11952,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>65</v>
       </c>
@@ -10568,7 +11986,7 @@
         <v>TP</v>
       </c>
       <c r="K69" s="2" t="str">
-        <f t="shared" ref="J69:V103" si="16">IF(AND(IF($D69&gt;=K$3,1,0)=1,$C69=1),"TP",IF(AND(IF($D69&gt;=K$3,1,0)=1,$C69=0),"FP",IF(AND(IF($D69&gt;=K$3,1,0)=0,$C69=0),"TN","FN")))</f>
+        <f t="shared" ref="K69:V87" si="16">IF(AND(IF($D69&gt;=K$3,1,0)=1,$C69=1),"TP",IF(AND(IF($D69&gt;=K$3,1,0)=1,$C69=0),"FP",IF(AND(IF($D69&gt;=K$3,1,0)=0,$C69=0),"TN","FN")))</f>
         <v>TP</v>
       </c>
       <c r="L69" s="2" t="str">
@@ -10616,7 +12034,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>66</v>
       </c>
@@ -10698,7 +12116,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>67</v>
       </c>
@@ -10780,7 +12198,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>68</v>
       </c>
@@ -10862,7 +12280,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>69</v>
       </c>
@@ -10944,7 +12362,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>70</v>
       </c>
@@ -11026,7 +12444,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>71</v>
       </c>
@@ -11108,7 +12526,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>72</v>
       </c>
@@ -11190,7 +12608,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>73</v>
       </c>
@@ -11272,7 +12690,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>74</v>
       </c>
@@ -11354,7 +12772,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>75</v>
       </c>
@@ -11436,7 +12854,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>76</v>
       </c>
@@ -11518,7 +12936,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>77</v>
       </c>
@@ -11600,7 +13018,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>78</v>
       </c>
@@ -11682,7 +13100,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>79</v>
       </c>
@@ -11764,7 +13182,7 @@
         <v>FP</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>80</v>
       </c>
@@ -11846,7 +13264,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>81</v>
       </c>
@@ -11928,7 +13346,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>82</v>
       </c>
@@ -12010,7 +13428,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>83</v>
       </c>
@@ -12092,7 +13510,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>84</v>
       </c>
@@ -12174,7 +13592,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>85</v>
       </c>
@@ -12256,7 +13674,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>86</v>
       </c>
@@ -12338,7 +13756,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>87</v>
       </c>
@@ -12420,7 +13838,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>88</v>
       </c>
@@ -12502,7 +13920,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>89</v>
       </c>
@@ -12584,7 +14002,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>90</v>
       </c>
@@ -12666,7 +14084,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>91</v>
       </c>
@@ -12748,7 +14166,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>92</v>
       </c>
@@ -12830,7 +14248,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>93</v>
       </c>
@@ -12912,7 +14330,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>94</v>
       </c>
@@ -12994,7 +14412,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>95</v>
       </c>
@@ -13076,7 +14494,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>96</v>
       </c>
@@ -13158,7 +14576,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>97</v>
       </c>
@@ -13240,7 +14658,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>98</v>
       </c>
@@ -13322,7 +14740,7 @@
         <v>TN</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>99</v>
       </c>
@@ -13404,7 +14822,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>3</v>
       </c>
@@ -13468,7 +14886,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>4</v>
       </c>
@@ -13531,7 +14949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I107" s="2" t="s">
         <v>4</v>
       </c>
@@ -13588,7 +15006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I108" s="2" t="s">
         <v>7</v>
       </c>
@@ -13645,7 +15063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J110" s="2" cm="1">
         <f t="array" ref="J110:V110">J3:V3</f>
         <v>0.375</v>
@@ -13687,7 +15105,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I112" s="2" t="s">
         <v>6</v>
       </c>
@@ -13744,7 +15162,7 @@
         <v>0.83018867924528306</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I113" s="2" t="s">
         <v>8</v>
       </c>
@@ -13801,7 +15219,7 @@
         <v>0.76595744680851063</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I114" s="2" t="s">
         <v>9</v>
       </c>
@@ -13858,7 +15276,7 @@
         <v>6.4231232436772423E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
@@ -13874,10 +15292,10 @@
       <c r="U115" s="2"/>
       <c r="V115" s="2"/>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H116" s="2"/>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
         <v>1</v>
       </c>
@@ -13888,7 +15306,7 @@
         <v>2</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>3</v>
@@ -13903,7 +15321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0</v>
       </c>
@@ -13937,7 +15355,7 @@
       </c>
       <c r="J119" s="1"/>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1</v>
       </c>
@@ -13971,7 +15389,7 @@
       </c>
       <c r="J120" s="1"/>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2</v>
       </c>
@@ -14005,7 +15423,7 @@
       </c>
       <c r="J121" s="1"/>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>3</v>
       </c>
@@ -14039,7 +15457,7 @@
       </c>
       <c r="J122" s="1"/>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>4</v>
       </c>
@@ -14073,7 +15491,7 @@
       </c>
       <c r="J123" s="1"/>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>5</v>
       </c>
@@ -14107,7 +15525,7 @@
       </c>
       <c r="J124" s="1"/>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>6</v>
       </c>
@@ -14141,7 +15559,7 @@
       </c>
       <c r="J125" s="1"/>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>7</v>
       </c>
@@ -14175,7 +15593,7 @@
       </c>
       <c r="J126" s="1"/>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>8</v>
       </c>
@@ -14209,7 +15627,7 @@
       </c>
       <c r="J127" s="1"/>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>9</v>
       </c>
@@ -14243,7 +15661,7 @@
       </c>
       <c r="J128" s="1"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>10</v>
       </c>
@@ -14277,7 +15695,7 @@
       </c>
       <c r="J129" s="1"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>11</v>
       </c>
@@ -14311,7 +15729,7 @@
       </c>
       <c r="J130" s="1"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>12</v>
       </c>
@@ -14345,7 +15763,7 @@
       </c>
       <c r="J131" s="1"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>13</v>
       </c>
@@ -14379,7 +15797,7 @@
       </c>
       <c r="J132" s="1"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>14</v>
       </c>
@@ -14413,7 +15831,7 @@
       </c>
       <c r="J133" s="1"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>15</v>
       </c>
@@ -14447,7 +15865,7 @@
       </c>
       <c r="J134" s="1"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>16</v>
       </c>
@@ -14481,7 +15899,7 @@
       </c>
       <c r="J135" s="1"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>17</v>
       </c>
@@ -14515,7 +15933,7 @@
       </c>
       <c r="J136" s="1"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>18</v>
       </c>
@@ -14549,7 +15967,7 @@
       </c>
       <c r="J137" s="1"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>19</v>
       </c>
@@ -14583,7 +16001,7 @@
       </c>
       <c r="J138" s="1"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>20</v>
       </c>
@@ -14617,7 +16035,7 @@
       </c>
       <c r="J139" s="1"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>21</v>
       </c>
@@ -14651,7 +16069,7 @@
       </c>
       <c r="J140" s="1"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>22</v>
       </c>
@@ -14685,7 +16103,7 @@
       </c>
       <c r="J141" s="1"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>23</v>
       </c>
@@ -14719,7 +16137,7 @@
       </c>
       <c r="J142" s="1"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>24</v>
       </c>
@@ -14753,7 +16171,7 @@
       </c>
       <c r="J143" s="1"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>25</v>
       </c>
@@ -14787,7 +16205,7 @@
       </c>
       <c r="J144" s="1"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>26</v>
       </c>
@@ -14821,7 +16239,7 @@
       </c>
       <c r="J145" s="1"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>27</v>
       </c>
@@ -14855,7 +16273,7 @@
       </c>
       <c r="J146" s="1"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>28</v>
       </c>
@@ -14889,7 +16307,7 @@
       </c>
       <c r="J147" s="1"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>29</v>
       </c>
@@ -14923,7 +16341,7 @@
       </c>
       <c r="J148" s="1"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>30</v>
       </c>
@@ -14957,7 +16375,7 @@
       </c>
       <c r="J149" s="1"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>31</v>
       </c>
@@ -14991,7 +16409,7 @@
       </c>
       <c r="J150" s="1"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>32</v>
       </c>
@@ -15025,7 +16443,7 @@
       </c>
       <c r="J151" s="1"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>33</v>
       </c>
@@ -15059,7 +16477,7 @@
       </c>
       <c r="J152" s="1"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>34</v>
       </c>
@@ -15093,7 +16511,7 @@
       </c>
       <c r="J153" s="1"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>35</v>
       </c>
@@ -15127,7 +16545,7 @@
       </c>
       <c r="J154" s="1"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>36</v>
       </c>
@@ -15161,7 +16579,7 @@
       </c>
       <c r="J155" s="1"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>37</v>
       </c>
@@ -15195,7 +16613,7 @@
       </c>
       <c r="J156" s="1"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>38</v>
       </c>
@@ -15229,7 +16647,7 @@
       </c>
       <c r="J157" s="1"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>39</v>
       </c>
@@ -15263,7 +16681,7 @@
       </c>
       <c r="J158" s="1"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>40</v>
       </c>
@@ -15297,7 +16715,7 @@
       </c>
       <c r="J159" s="1"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>41</v>
       </c>
@@ -15331,7 +16749,7 @@
       </c>
       <c r="J160" s="1"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>42</v>
       </c>
@@ -15365,7 +16783,7 @@
       </c>
       <c r="J161" s="1"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>43</v>
       </c>
@@ -15399,7 +16817,7 @@
       </c>
       <c r="J162" s="1"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>44</v>
       </c>
@@ -15433,7 +16851,7 @@
       </c>
       <c r="J163" s="1"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>45</v>
       </c>
@@ -15467,7 +16885,7 @@
       </c>
       <c r="J164" s="1"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>46</v>
       </c>
@@ -15501,7 +16919,7 @@
       </c>
       <c r="J165" s="1"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>47</v>
       </c>
@@ -15535,7 +16953,7 @@
       </c>
       <c r="J166" s="1"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>48</v>
       </c>
@@ -15569,7 +16987,7 @@
       </c>
       <c r="J167" s="1"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>49</v>
       </c>
@@ -15603,7 +17021,7 @@
       </c>
       <c r="J168" s="1"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>50</v>
       </c>
@@ -15637,7 +17055,7 @@
       </c>
       <c r="J169" s="1"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>51</v>
       </c>
@@ -15671,7 +17089,7 @@
       </c>
       <c r="J170" s="1"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>52</v>
       </c>
@@ -15705,7 +17123,7 @@
       </c>
       <c r="J171" s="1"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>53</v>
       </c>
@@ -15739,7 +17157,7 @@
       </c>
       <c r="J172" s="1"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>54</v>
       </c>
@@ -15773,7 +17191,7 @@
       </c>
       <c r="J173" s="1"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>55</v>
       </c>
@@ -15807,7 +17225,7 @@
       </c>
       <c r="J174" s="1"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>56</v>
       </c>
@@ -15841,7 +17259,7 @@
       </c>
       <c r="J175" s="1"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>57</v>
       </c>
@@ -15875,7 +17293,7 @@
       </c>
       <c r="J176" s="1"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>58</v>
       </c>
@@ -15909,7 +17327,7 @@
       </c>
       <c r="J177" s="1"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>59</v>
       </c>
@@ -15943,7 +17361,7 @@
       </c>
       <c r="J178" s="1"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>60</v>
       </c>
@@ -15977,7 +17395,7 @@
       </c>
       <c r="J179" s="1"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>61</v>
       </c>
@@ -16011,7 +17429,7 @@
       </c>
       <c r="J180" s="1"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>62</v>
       </c>
@@ -16045,7 +17463,7 @@
       </c>
       <c r="J181" s="1"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>63</v>
       </c>
@@ -16079,7 +17497,7 @@
       </c>
       <c r="J182" s="1"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>64</v>
       </c>
@@ -16113,7 +17531,7 @@
       </c>
       <c r="J183" s="1"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>65</v>
       </c>
@@ -16147,7 +17565,7 @@
       </c>
       <c r="J184" s="1"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>66</v>
       </c>
@@ -16181,7 +17599,7 @@
       </c>
       <c r="J185" s="1"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>67</v>
       </c>
@@ -16215,7 +17633,7 @@
       </c>
       <c r="J186" s="1"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>68</v>
       </c>
@@ -16249,7 +17667,7 @@
       </c>
       <c r="J187" s="1"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>69</v>
       </c>
@@ -16283,7 +17701,7 @@
       </c>
       <c r="J188" s="1"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>70</v>
       </c>
@@ -16317,7 +17735,7 @@
       </c>
       <c r="J189" s="1"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>71</v>
       </c>
@@ -16351,7 +17769,7 @@
       </c>
       <c r="J190" s="1"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>72</v>
       </c>
@@ -16385,7 +17803,7 @@
       </c>
       <c r="J191" s="1"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>73</v>
       </c>
@@ -16419,7 +17837,7 @@
       </c>
       <c r="J192" s="1"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>74</v>
       </c>
@@ -16453,7 +17871,7 @@
       </c>
       <c r="J193" s="1"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>75</v>
       </c>
@@ -16487,7 +17905,7 @@
       </c>
       <c r="J194" s="1"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>76</v>
       </c>
@@ -16521,7 +17939,7 @@
       </c>
       <c r="J195" s="1"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>77</v>
       </c>
@@ -16555,7 +17973,7 @@
       </c>
       <c r="J196" s="1"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>78</v>
       </c>
@@ -16589,7 +18007,7 @@
       </c>
       <c r="J197" s="1"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>79</v>
       </c>
@@ -16623,7 +18041,7 @@
       </c>
       <c r="J198" s="1"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>80</v>
       </c>
@@ -16657,7 +18075,7 @@
       </c>
       <c r="J199" s="1"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>81</v>
       </c>
@@ -16691,7 +18109,7 @@
       </c>
       <c r="J200" s="1"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>82</v>
       </c>
@@ -16725,7 +18143,7 @@
       </c>
       <c r="J201" s="1"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>83</v>
       </c>
@@ -16759,7 +18177,7 @@
       </c>
       <c r="J202" s="1"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>84</v>
       </c>
@@ -16793,7 +18211,7 @@
       </c>
       <c r="J203" s="1"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>85</v>
       </c>
@@ -16827,7 +18245,7 @@
       </c>
       <c r="J204" s="1"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>86</v>
       </c>
@@ -16861,7 +18279,7 @@
       </c>
       <c r="J205" s="1"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>87</v>
       </c>
@@ -16895,7 +18313,7 @@
       </c>
       <c r="J206" s="1"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>88</v>
       </c>
@@ -16929,7 +18347,7 @@
       </c>
       <c r="J207" s="1"/>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>89</v>
       </c>
@@ -16963,7 +18381,7 @@
       </c>
       <c r="J208" s="1"/>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>90</v>
       </c>
@@ -16997,7 +18415,7 @@
       </c>
       <c r="J209" s="1"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>91</v>
       </c>
@@ -17031,7 +18449,7 @@
       </c>
       <c r="J210" s="1"/>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>92</v>
       </c>
@@ -17065,7 +18483,7 @@
       </c>
       <c r="J211" s="1"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>93</v>
       </c>
@@ -17099,7 +18517,7 @@
       </c>
       <c r="J212" s="1"/>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>94</v>
       </c>
@@ -17133,7 +18551,7 @@
       </c>
       <c r="J213" s="1"/>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>95</v>
       </c>
@@ -17167,7 +18585,7 @@
       </c>
       <c r="J214" s="1"/>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>96</v>
       </c>
@@ -17201,7 +18619,7 @@
       </c>
       <c r="J215" s="1"/>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>97</v>
       </c>
@@ -17235,7 +18653,7 @@
       </c>
       <c r="J216" s="1"/>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>98</v>
       </c>
@@ -17269,7 +18687,7 @@
       </c>
       <c r="J217" s="1"/>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>99</v>
       </c>
@@ -17303,10 +18721,10 @@
       </c>
       <c r="J218" s="1"/>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E219" s="2"/>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E220" s="2"/>
     </row>
   </sheetData>

</xml_diff>